<commit_message>
fix: change to recall and precision
</commit_message>
<xml_diff>
--- a/experiments/node_results.xlsx
+++ b/experiments/node_results.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinsz\Desktop\NLP_project\03code\IDExtraction\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97B68B0-6BF3-413C-B1E1-8970814D59C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9BB9B0-36E5-4D2D-9170-B06AF1A046A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>nodes_0shot_0</t>
   </si>
@@ -53,13 +62,25 @@
   <si>
     <t>zs_cot</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_recall</t>
+  </si>
+  <si>
+    <t>name_precision</t>
+  </si>
+  <si>
+    <t>value_recall</t>
+  </si>
+  <si>
+    <t>value_precision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +95,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -83,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,14 +119,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -380,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -392,9 +438,10 @@
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="6" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -405,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -419,7 +466,7 @@
         <v>0.89750732</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -433,7 +480,7 @@
         <v>0.91570349799999995</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -447,7 +494,7 @@
         <v>0.91569193999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -461,7 +508,7 @@
         <v>0.92706503299999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -475,7 +522,7 @@
         <v>0.85005008500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -487,6 +534,143 @@
       </c>
       <c r="D7" s="1">
         <v>0.84785213400000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0.73373401140391403</v>
+      </c>
+      <c r="C10">
+        <v>0.79257589767298475</v>
+      </c>
+      <c r="D10">
+        <v>0.71558021266759109</v>
+      </c>
+      <c r="E10">
+        <v>0.86812297734627841</v>
+      </c>
+      <c r="F10">
+        <v>0.89158576051779947</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>0.77297349360456169</v>
+      </c>
+      <c r="C11">
+        <v>0.81281399291108025</v>
+      </c>
+      <c r="D11">
+        <v>0.6920711974110032</v>
+      </c>
+      <c r="E11">
+        <v>0.91100323624595481</v>
+      </c>
+      <c r="F11">
+        <v>0.92071197411003247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0.83350670365233437</v>
+      </c>
+      <c r="C12">
+        <v>0.76533329130416505</v>
+      </c>
+      <c r="D12">
+        <v>0.67102018801047913</v>
+      </c>
+      <c r="E12">
+        <v>0.89482200647249199</v>
+      </c>
+      <c r="F12">
+        <v>0.89482200647249199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>0.84985745107104316</v>
+      </c>
+      <c r="C13">
+        <v>0.74554391132061015</v>
+      </c>
+      <c r="D13">
+        <v>0.74323470488519039</v>
+      </c>
+      <c r="E13">
+        <v>0.92233009708737879</v>
+      </c>
+      <c r="F13">
+        <v>0.91747572815533984</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0.80248112189859744</v>
+      </c>
+      <c r="C14">
+        <v>0.7348120595693407</v>
+      </c>
+      <c r="D14">
+        <v>0.66680536292186776</v>
+      </c>
+      <c r="E14">
+        <v>0.85760517799352742</v>
+      </c>
+      <c r="F14">
+        <v>0.88025889967637549</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>0.59940668824163978</v>
+      </c>
+      <c r="C15">
+        <v>0.79729542302357803</v>
+      </c>
+      <c r="D15">
+        <v>0.5553513638465094</v>
+      </c>
+      <c r="E15">
+        <v>0.85760517799352742</v>
+      </c>
+      <c r="F15">
+        <v>0.87378640776699024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>